<commit_message>
Correction d'un petit bug sur l'échange avec une meringue
</commit_message>
<xml_diff>
--- a/2018-2019/L2 INFO/BPOO/ProjetBPOO2018-2019/plateaux/plateauModele.xlsx
+++ b/2018-2019/L2 INFO/BPOO/ProjetBPOO2018-2019/plateaux/plateauModele.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="plateau1.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -106,7 +106,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -186,795 +186,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF8000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0080FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF008000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1307,7 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1358,15 +569,15 @@
       </c>
       <c r="N4">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:W13" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
@@ -1378,11 +589,11 @@
       </c>
       <c r="S4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
@@ -1390,11 +601,11 @@
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -1434,19 +645,19 @@
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="0"/>
@@ -1454,7 +665,7 @@
       </c>
       <c r="T5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <f t="shared" ca="1" si="0"/>
@@ -1462,7 +673,7 @@
       </c>
       <c r="V5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <f t="shared" ca="1" si="0"/>
@@ -1502,19 +713,19 @@
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="0"/>
@@ -1522,23 +733,23 @@
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -1574,15 +785,15 @@
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="0"/>
@@ -1598,7 +809,7 @@
       </c>
       <c r="T7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U7">
         <f t="shared" ca="1" si="0"/>
@@ -1606,11 +817,11 @@
       </c>
       <c r="V7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -1646,43 +857,43 @@
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -1726,7 +937,7 @@
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="0"/>
@@ -1734,27 +945,27 @@
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -1790,7 +1001,7 @@
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="0"/>
@@ -1798,35 +1009,35 @@
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -1866,7 +1077,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P11">
         <f t="shared" ca="1" si="0"/>
@@ -1882,23 +1093,23 @@
       </c>
       <c r="S11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -1934,11 +1145,11 @@
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="0"/>
@@ -1946,7 +1157,7 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="0"/>
@@ -1958,7 +1169,7 @@
       </c>
       <c r="T12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U12">
         <f t="shared" ca="1" si="0"/>
@@ -1966,11 +1177,11 @@
       </c>
       <c r="V12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -2006,15 +1217,15 @@
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="0"/>
@@ -2022,7 +1233,7 @@
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="0"/>
@@ -2030,52 +1241,51 @@
       </c>
       <c r="T13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:J13">
-    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:W13">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",N4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",N4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",N4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",N4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>